<commit_message>
Add a Second Test Case
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Documents\App project RES NOVAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB328FC7-F536-46B5-8F92-D4039AE4EA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729BDED-B60E-445C-9C92-CCCA590B50C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -95,6 +95,24 @@
   </si>
   <si>
     <t>See if the returned binary number is correct</t>
+  </si>
+  <si>
+    <t>binToGraysCode</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>The function should return the given binary number in its gray code representation</t>
+  </si>
+  <si>
+    <t>See if the returned gray code number is correct</t>
+  </si>
+  <si>
+    <t>Input a binary number</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function binToGraysCode</t>
   </si>
 </sst>
 </file>
@@ -294,17 +312,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -313,55 +355,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -686,7 +710,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,49 +723,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -753,22 +777,22 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="1"/>
@@ -777,22 +801,22 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1"/>
@@ -801,64 +825,64 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="13" t="s">
+    <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+    <row r="15" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -869,6 +893,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="F10:F15"/>
     <mergeCell ref="E10:E15"/>
@@ -877,11 +906,6 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -890,12 +914,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE54753-D611-4146-9A52-A54D3D4605A3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="1:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add another Test Case in the Test Cases file
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729BDED-B60E-445C-9C92-CCCA590B50C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E43183-7D2E-4512-BBF8-58AF7FC04600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -113,6 +114,21 @@
   </si>
   <si>
     <t>This test case checks the functionality of the function binToGraysCode</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>grayCodeConversion</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function grayCodeConversion</t>
+  </si>
+  <si>
+    <t>The function should return the given decimal number in its gray code representation</t>
   </si>
 </sst>
 </file>
@@ -312,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -322,6 +338,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,6 +392,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,6 +409,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -709,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D230F1F-2D54-4C7D-BA37-BB5E26089A3D}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -723,49 +749,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -801,22 +827,22 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1"/>
@@ -825,64 +851,64 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="8" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="8" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -917,7 +943,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+      <selection activeCell="D10" sqref="D10:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,46 +957,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -989,73 +1015,73 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+    <row r="11" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1074,4 +1100,172 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85C9A7B-C2AD-44C0-8615-808F759A96F7}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Test Case about checkDay function
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E43183-7D2E-4512-BBF8-58AF7FC04600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178C5552-64BE-41A9-B6B8-4D7EB290B256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -129,6 +130,34 @@
   </si>
   <si>
     <t>The function should return the given decimal number in its gray code representation</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>checkDay</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function checkDay</t>
+  </si>
+  <si>
+    <t>Input two decimal number</t>
+  </si>
+  <si>
+    <t>Check if the function takes the given numbers</t>
+  </si>
+  <si>
+    <t>Check whether the input is correct</t>
+  </si>
+  <si>
+    <t>See if the returned number is correct</t>
+  </si>
+  <si>
+    <t>The function should return the given date if the inputed numbers are valid</t>
+  </si>
+  <si>
+    <t>Completed 
+manually</t>
   </si>
 </sst>
 </file>
@@ -328,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -338,81 +367,84 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,49 +781,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -827,22 +859,22 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1"/>
@@ -851,64 +883,64 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -919,11 +951,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="F10:F15"/>
     <mergeCell ref="E10:E15"/>
@@ -932,6 +959,11 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -957,34 +989,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1015,73 +1047,73 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="24" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1106,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85C9A7B-C2AD-44C0-8615-808F759A96F7}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,37 +1152,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="30"/>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="30"/>
@@ -1163,92 +1195,92 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="24" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
-      <c r="F16" s="23"/>
+      <c r="F16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1268,4 +1300,174 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A304EA-CC30-4B02-8C35-6E3815D11894}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Test Case about checkYear function
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178C5552-64BE-41A9-B6B8-4D7EB290B256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4078681-80BE-405C-BF40-DC396F4DBB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -158,6 +159,24 @@
   <si>
     <t>Completed 
 manually</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function checkYear</t>
+  </si>
+  <si>
+    <t>checkYear</t>
+  </si>
+  <si>
+    <t>Verify that the function complete all the checks correctly</t>
+  </si>
+  <si>
+    <t>The function should complete all the checks and return the checked data</t>
+  </si>
+  <si>
+    <t>Completed manually</t>
   </si>
 </sst>
 </file>
@@ -357,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -370,7 +389,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,49 +812,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -859,22 +890,22 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="28" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1"/>
@@ -883,64 +914,64 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -975,7 +1006,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D15"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,46 +1020,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1047,73 +1078,73 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1152,46 +1183,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1207,80 +1238,80 @@
       <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1306,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A304EA-CC30-4B02-8C35-6E3815D11894}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,50 +1351,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1382,75 +1413,75 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="31" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1470,4 +1501,154 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3AADC2-47EB-4F7C-9582-504AAE921B69}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="29"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="29"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="E10:E14"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="D10:D14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a Test Case about checkMonth function
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4078681-80BE-405C-BF40-DC396F4DBB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E4BD5C-04B1-4016-9E34-AF85C6B0F906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -177,6 +178,15 @@
   </si>
   <si>
     <t>Completed manually</t>
+  </si>
+  <si>
+    <t>checkMonth</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function checkMonth</t>
   </si>
 </sst>
 </file>
@@ -376,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -389,19 +399,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,24 +430,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -462,20 +448,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,7 +800,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,49 +813,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -890,22 +891,22 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1"/>
@@ -914,64 +915,64 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="28" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1006,7 +1007,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,46 +1021,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1078,73 +1079,73 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="28" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1170,7 +1171,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,46 +1184,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1238,80 +1239,80 @@
       <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="28" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1338,7 +1339,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,50 +1352,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1413,75 +1414,75 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="35" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1507,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3AADC2-47EB-4F7C-9582-504AAE921B69}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,53 +1522,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1576,64 +1577,64 @@
       <c r="D9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="29"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="29"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="29"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="30"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1651,4 +1652,166 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D64020-E7EC-4D68-A707-294890E3EFA6}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a Test Case about checkBigger function
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E4BD5C-04B1-4016-9E34-AF85C6B0F906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559A38B9-A355-4EA0-A4A7-B4AA80ACE894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
     <sheet name="Лист6" sheetId="6" r:id="rId6"/>
+    <sheet name="Лист7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -187,6 +188,24 @@
   </si>
   <si>
     <t>This test case checks the functionality of the function checkMonth</t>
+  </si>
+  <si>
+    <t>checkBigger</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function checkBigger</t>
+  </si>
+  <si>
+    <t>Check if the function takes the input</t>
+  </si>
+  <si>
+    <t>See if the function returns a result of type boolean</t>
+  </si>
+  <si>
+    <t>The function takes the given input, does all the check and returns a result of type boolean</t>
   </si>
 </sst>
 </file>
@@ -386,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -476,6 +495,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1658,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D64020-E7EC-4D68-A707-294890E3EFA6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,4 +1848,170 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FCD911-157E-4A87-A78A-0B7141792540}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Test Case about getGrayCode function
</commit_message>
<xml_diff>
--- a/QA documentation/Test Cases.xlsx
+++ b/QA documentation/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\res-novas\QA documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559A38B9-A355-4EA0-A4A7-B4AA80ACE894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039EDC43-9888-4C64-A954-BA7FC2A56D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{25CD6D35-0B77-4F05-9110-B41665BB5183}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
     <sheet name="Лист6" sheetId="6" r:id="rId6"/>
     <sheet name="Лист7" sheetId="7" r:id="rId7"/>
+    <sheet name="Лист8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -206,6 +207,24 @@
   </si>
   <si>
     <t>The function takes the given input, does all the check and returns a result of type boolean</t>
+  </si>
+  <si>
+    <t>getGrayCode</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>This test case checks the functionality of the function getGrayCode</t>
+  </si>
+  <si>
+    <t>Check if the function takes the input data</t>
+  </si>
+  <si>
+    <t>Check if the function successfully converts the input into uniqe gray code</t>
+  </si>
+  <si>
+    <t>The function takes the given input, and converts it into uniqe grey code</t>
   </si>
 </sst>
 </file>
@@ -1854,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FCD911-157E-4A87-A78A-0B7141792540}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,4 +2033,165 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D579999B-ED24-49E4-B4AD-4EF2E6BF2724}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>